<commit_message>
Set up for Foreign Fighters & Muslims
</commit_message>
<xml_diff>
--- a/assignment_2/Foreign_Fighters.xlsx
+++ b/assignment_2/Foreign_Fighters.xlsx
@@ -108,9 +108,6 @@
     <t>Luxembourg</t>
   </si>
   <si>
-    <t>Macedonia, FYR</t>
-  </si>
-  <si>
     <t>Malta</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>Foreign_Fighters</t>
+  </si>
+  <si>
+    <t>Macedonia FYR</t>
   </si>
 </sst>
 </file>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,10 +503,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -551,7 +551,7 @@
     </row>
     <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="3">
         <v>340</v>
@@ -561,7 +561,7 @@
     </row>
     <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="3">
         <v>7</v>
@@ -740,7 +740,7 @@
     </row>
     <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B25" s="3">
         <v>24</v>
@@ -750,7 +750,7 @@
     </row>
     <row r="26" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -760,7 +760,7 @@
     </row>
     <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="1">
         <v>4</v>
@@ -790,7 +790,7 @@
     </row>
     <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1">
         <v>40</v>
@@ -800,7 +800,7 @@
     </row>
     <row r="31" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1">
         <v>12</v>
@@ -810,7 +810,7 @@
     </row>
     <row r="32" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1">
         <v>70</v>
@@ -820,7 +820,7 @@
     </row>
     <row r="33" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1">
         <v>6</v>
@@ -830,7 +830,7 @@
     </row>
     <row r="34" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="3">
         <v>3</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="38" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38" s="3">
         <v>45</v>

</xml_diff>